<commit_message>
SSA básico con ajuste sobre parámetros óptimo
</commit_message>
<xml_diff>
--- a/results_SSA_py/results_cec2017_10.xlsx
+++ b/results_SSA_py/results_cec2017_10.xlsx
@@ -603,94 +603,94 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>5420793000</v>
+        <v>1506942000</v>
       </c>
       <c r="D2" t="n">
-        <v>964669400</v>
+        <v>3581715</v>
       </c>
       <c r="E2" t="n">
-        <v>11633.56</v>
+        <v>6530.364</v>
       </c>
       <c r="F2" t="n">
-        <v>248.8578</v>
+        <v>157.6725</v>
       </c>
       <c r="G2" t="n">
-        <v>86.35599999999999</v>
+        <v>50.177</v>
       </c>
       <c r="H2" t="n">
-        <v>36.27352</v>
+        <v>46.61102</v>
       </c>
       <c r="I2" t="n">
-        <v>59.69333</v>
+        <v>73.04996</v>
       </c>
       <c r="J2" t="n">
-        <v>46.6728</v>
+        <v>25.20236</v>
       </c>
       <c r="K2" t="n">
-        <v>325.2144</v>
+        <v>456.8864</v>
       </c>
       <c r="L2" t="n">
-        <v>2479.686</v>
+        <v>1502.914</v>
       </c>
       <c r="M2" t="n">
-        <v>1041.993</v>
+        <v>118.8025</v>
       </c>
       <c r="N2" t="n">
-        <v>6937862</v>
+        <v>8465174</v>
       </c>
       <c r="O2" t="n">
-        <v>10764.02</v>
+        <v>14506.3</v>
       </c>
       <c r="P2" t="n">
-        <v>3664.283</v>
+        <v>426.1636</v>
       </c>
       <c r="Q2" t="n">
-        <v>6906.808</v>
+        <v>2143.902</v>
       </c>
       <c r="R2" t="n">
-        <v>267.8599</v>
+        <v>461.7841</v>
       </c>
       <c r="S2" t="n">
-        <v>92.08839999999999</v>
+        <v>174.2534</v>
       </c>
       <c r="T2" t="n">
-        <v>12038240</v>
+        <v>9613.839</v>
       </c>
       <c r="U2" t="n">
-        <v>58792.67</v>
+        <v>6322.554</v>
       </c>
       <c r="V2" t="n">
-        <v>254.664</v>
+        <v>71.46211</v>
       </c>
       <c r="W2" t="n">
-        <v>195.6077</v>
+        <v>246.9401</v>
       </c>
       <c r="X2" t="n">
-        <v>302.0807</v>
+        <v>260.325</v>
       </c>
       <c r="Y2" t="n">
-        <v>466.9398</v>
+        <v>390.2243</v>
       </c>
       <c r="Z2" t="n">
-        <v>316.5707</v>
+        <v>486.1137</v>
       </c>
       <c r="AA2" t="n">
-        <v>452.4674</v>
+        <v>523.4447</v>
       </c>
       <c r="AB2" t="n">
-        <v>1104.643</v>
+        <v>548.7572</v>
       </c>
       <c r="AC2" t="n">
-        <v>585.8551</v>
+        <v>433.7112</v>
       </c>
       <c r="AD2" t="n">
-        <v>733.4258</v>
+        <v>688.9903</v>
       </c>
       <c r="AE2" t="n">
-        <v>296.6269</v>
+        <v>432.8603</v>
       </c>
       <c r="AF2" t="n">
-        <v>27051050</v>
+        <v>4897171</v>
       </c>
       <c r="AG2" t="n">
         <v>10</v>
@@ -704,94 +704,94 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>3167039000</v>
+        <v>144161600</v>
       </c>
       <c r="D3" t="n">
-        <v>146442000</v>
+        <v>2148565</v>
       </c>
       <c r="E3" t="n">
-        <v>6630.184</v>
+        <v>5371.355</v>
       </c>
       <c r="F3" t="n">
-        <v>189.2191</v>
+        <v>72.06381</v>
       </c>
       <c r="G3" t="n">
-        <v>85.81229999999999</v>
+        <v>40.5705</v>
       </c>
       <c r="H3" t="n">
-        <v>31.99896</v>
+        <v>45.90763</v>
       </c>
       <c r="I3" t="n">
-        <v>46.63778</v>
+        <v>70.80725</v>
       </c>
       <c r="J3" t="n">
-        <v>44.35143</v>
+        <v>12.10798</v>
       </c>
       <c r="K3" t="n">
-        <v>276.2079</v>
+        <v>417.7699</v>
       </c>
       <c r="L3" t="n">
-        <v>2138.754</v>
+        <v>1129.159</v>
       </c>
       <c r="M3" t="n">
-        <v>483.4966</v>
+        <v>56.63853</v>
       </c>
       <c r="N3" t="n">
-        <v>558609.8</v>
+        <v>6883668</v>
       </c>
       <c r="O3" t="n">
-        <v>10762.76</v>
+        <v>14502.32</v>
       </c>
       <c r="P3" t="n">
-        <v>3664.18</v>
+        <v>426.0984</v>
       </c>
       <c r="Q3" t="n">
-        <v>6894.504</v>
+        <v>2142.548</v>
       </c>
       <c r="R3" t="n">
-        <v>259.7421</v>
+        <v>441.4269</v>
       </c>
       <c r="S3" t="n">
-        <v>76.62945000000001</v>
+        <v>150.5209</v>
       </c>
       <c r="T3" t="n">
-        <v>678563.6</v>
+        <v>9613.404</v>
       </c>
       <c r="U3" t="n">
-        <v>58642.85</v>
+        <v>6307.875</v>
       </c>
       <c r="V3" t="n">
-        <v>251.9601</v>
+        <v>54.81747</v>
       </c>
       <c r="W3" t="n">
-        <v>173.9178</v>
+        <v>240.1499</v>
       </c>
       <c r="X3" t="n">
-        <v>241.9449</v>
+        <v>81.86485</v>
       </c>
       <c r="Y3" t="n">
-        <v>405.4309</v>
+        <v>382.4629</v>
       </c>
       <c r="Z3" t="n">
-        <v>228.1761</v>
+        <v>478.3026</v>
       </c>
       <c r="AA3" t="n">
-        <v>449.4254</v>
+        <v>476.6529</v>
       </c>
       <c r="AB3" t="n">
-        <v>1019.032</v>
+        <v>378.3701</v>
       </c>
       <c r="AC3" t="n">
-        <v>578.0909</v>
+        <v>430.8472</v>
       </c>
       <c r="AD3" t="n">
-        <v>614.2254</v>
+        <v>655.4406</v>
       </c>
       <c r="AE3" t="n">
-        <v>293.6155</v>
+        <v>418.0295</v>
       </c>
       <c r="AF3" t="n">
-        <v>26374300</v>
+        <v>4167982</v>
       </c>
       <c r="AG3" t="n">
         <v>10</v>
@@ -805,94 +805,94 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>2982803000</v>
+        <v>23814720</v>
       </c>
       <c r="D4" t="n">
-        <v>64182750</v>
+        <v>1203143</v>
       </c>
       <c r="E4" t="n">
-        <v>4860.302</v>
+        <v>3140.733</v>
       </c>
       <c r="F4" t="n">
-        <v>153.7326</v>
+        <v>68.74303</v>
       </c>
       <c r="G4" t="n">
-        <v>85.30463</v>
+        <v>39.98915</v>
       </c>
       <c r="H4" t="n">
-        <v>30.83589</v>
+        <v>45.49082</v>
       </c>
       <c r="I4" t="n">
-        <v>44.47954</v>
+        <v>70.27233</v>
       </c>
       <c r="J4" t="n">
-        <v>43.10632</v>
+        <v>11.08265</v>
       </c>
       <c r="K4" t="n">
-        <v>253.8336</v>
+        <v>395.6067</v>
       </c>
       <c r="L4" t="n">
-        <v>2107.498</v>
+        <v>1054.52</v>
       </c>
       <c r="M4" t="n">
-        <v>393.3254</v>
+        <v>34.90727</v>
       </c>
       <c r="N4" t="n">
-        <v>97542.61</v>
+        <v>6741261</v>
       </c>
       <c r="O4" t="n">
-        <v>10761.57</v>
+        <v>14495.23</v>
       </c>
       <c r="P4" t="n">
-        <v>3661.639</v>
+        <v>425.9978</v>
       </c>
       <c r="Q4" t="n">
-        <v>6894.464</v>
+        <v>796.3069</v>
       </c>
       <c r="R4" t="n">
-        <v>259.5036</v>
+        <v>424.24</v>
       </c>
       <c r="S4" t="n">
-        <v>74.24659</v>
+        <v>148.1752</v>
       </c>
       <c r="T4" t="n">
-        <v>516333.4</v>
+        <v>9613.01</v>
       </c>
       <c r="U4" t="n">
-        <v>58350.92</v>
+        <v>6048.948</v>
       </c>
       <c r="V4" t="n">
-        <v>251.0909</v>
+        <v>51.38461</v>
       </c>
       <c r="W4" t="n">
-        <v>131.3123</v>
+        <v>237.828</v>
       </c>
       <c r="X4" t="n">
-        <v>205.5224</v>
+        <v>56.44933</v>
       </c>
       <c r="Y4" t="n">
-        <v>401.1606</v>
+        <v>382.0984</v>
       </c>
       <c r="Z4" t="n">
-        <v>189.6667</v>
+        <v>476.4027</v>
       </c>
       <c r="AA4" t="n">
-        <v>449.369</v>
+        <v>458.4586</v>
       </c>
       <c r="AB4" t="n">
-        <v>1013.111</v>
+        <v>256.3658</v>
       </c>
       <c r="AC4" t="n">
-        <v>577.3992</v>
+        <v>430.1976</v>
       </c>
       <c r="AD4" t="n">
-        <v>519.263</v>
+        <v>628.6345</v>
       </c>
       <c r="AE4" t="n">
-        <v>293.3028</v>
+        <v>415.6058</v>
       </c>
       <c r="AF4" t="n">
-        <v>13896650</v>
+        <v>4103641</v>
       </c>
       <c r="AG4" t="n">
         <v>10</v>
@@ -906,94 +906,94 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>2775703000</v>
+        <v>809442.6</v>
       </c>
       <c r="D5" t="n">
-        <v>15597000</v>
+        <v>793467</v>
       </c>
       <c r="E5" t="n">
-        <v>2477.808</v>
+        <v>741.4162</v>
       </c>
       <c r="F5" t="n">
-        <v>133.0508</v>
+        <v>67.29107</v>
       </c>
       <c r="G5" t="n">
-        <v>80.59672</v>
+        <v>39.80505</v>
       </c>
       <c r="H5" t="n">
-        <v>30.17206</v>
+        <v>45.01955</v>
       </c>
       <c r="I5" t="n">
-        <v>43.53799</v>
+        <v>69.92425</v>
       </c>
       <c r="J5" t="n">
-        <v>41.4086</v>
+        <v>10.95159</v>
       </c>
       <c r="K5" t="n">
-        <v>241.954</v>
+        <v>377.7705</v>
       </c>
       <c r="L5" t="n">
-        <v>1716.031</v>
+        <v>1034.439</v>
       </c>
       <c r="M5" t="n">
-        <v>262.9212</v>
+        <v>30.1989</v>
       </c>
       <c r="N5" t="n">
-        <v>45674.1</v>
+        <v>6533971</v>
       </c>
       <c r="O5" t="n">
-        <v>10758.69</v>
+        <v>14400.67</v>
       </c>
       <c r="P5" t="n">
-        <v>3660.799</v>
+        <v>267.7394</v>
       </c>
       <c r="Q5" t="n">
-        <v>6685.786</v>
+        <v>795.2224</v>
       </c>
       <c r="R5" t="n">
-        <v>256.8355</v>
+        <v>417.3957</v>
       </c>
       <c r="S5" t="n">
-        <v>73.6703</v>
+        <v>141.2627</v>
       </c>
       <c r="T5" t="n">
-        <v>55400.94</v>
+        <v>9605.98</v>
       </c>
       <c r="U5" t="n">
-        <v>54254.72</v>
+        <v>4882.848</v>
       </c>
       <c r="V5" t="n">
-        <v>250.4858</v>
+        <v>49.84647</v>
       </c>
       <c r="W5" t="n">
-        <v>130.4731</v>
+        <v>237.1915</v>
       </c>
       <c r="X5" t="n">
-        <v>198.9297</v>
+        <v>46.25453</v>
       </c>
       <c r="Y5" t="n">
-        <v>393.6349</v>
+        <v>381.6947</v>
       </c>
       <c r="Z5" t="n">
-        <v>181.0039</v>
+        <v>416.3205</v>
       </c>
       <c r="AA5" t="n">
-        <v>446.3293</v>
+        <v>449.4754</v>
       </c>
       <c r="AB5" t="n">
-        <v>1005.974</v>
+        <v>222.9816</v>
       </c>
       <c r="AC5" t="n">
-        <v>577.3753</v>
+        <v>430.1645</v>
       </c>
       <c r="AD5" t="n">
-        <v>461.6947</v>
+        <v>609.5723</v>
       </c>
       <c r="AE5" t="n">
-        <v>293.1529</v>
+        <v>403.8849</v>
       </c>
       <c r="AF5" t="n">
-        <v>2096605</v>
+        <v>4067446</v>
       </c>
       <c r="AG5" t="n">
         <v>10</v>
@@ -1007,94 +1007,94 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>1635053000</v>
+        <v>1697.685</v>
       </c>
       <c r="D6" t="n">
-        <v>3565547</v>
+        <v>162023</v>
       </c>
       <c r="E6" t="n">
-        <v>1835.986</v>
+        <v>150.4513</v>
       </c>
       <c r="F6" t="n">
-        <v>85.03016</v>
+        <v>66.33759000000001</v>
       </c>
       <c r="G6" t="n">
-        <v>71.86863</v>
+        <v>39.79835</v>
       </c>
       <c r="H6" t="n">
-        <v>29.98059</v>
+        <v>44.38858</v>
       </c>
       <c r="I6" t="n">
-        <v>42.82055</v>
+        <v>69.90085000000001</v>
       </c>
       <c r="J6" t="n">
-        <v>13.07818</v>
+        <v>10.94455</v>
       </c>
       <c r="K6" t="n">
-        <v>238.3421</v>
+        <v>376.0787</v>
       </c>
       <c r="L6" t="n">
-        <v>1625.411</v>
+        <v>1032.01</v>
       </c>
       <c r="M6" t="n">
-        <v>73.92100000000001</v>
+        <v>25.91306</v>
       </c>
       <c r="N6" t="n">
-        <v>13433.49</v>
+        <v>6039782</v>
       </c>
       <c r="O6" t="n">
-        <v>10753.23</v>
+        <v>14341.03</v>
       </c>
       <c r="P6" t="n">
-        <v>3542.553</v>
+        <v>121.885</v>
       </c>
       <c r="Q6" t="n">
-        <v>5924.158</v>
+        <v>784.6626</v>
       </c>
       <c r="R6" t="n">
-        <v>252.9481</v>
+        <v>414.9629</v>
       </c>
       <c r="S6" t="n">
-        <v>72.48716</v>
+        <v>140.7251</v>
       </c>
       <c r="T6" t="n">
-        <v>1386.914</v>
+        <v>9603.837</v>
       </c>
       <c r="U6" t="n">
-        <v>10406.9</v>
+        <v>4737.081</v>
       </c>
       <c r="V6" t="n">
-        <v>249.2634</v>
+        <v>46.88336</v>
       </c>
       <c r="W6" t="n">
-        <v>121.2843</v>
+        <v>237.1397</v>
       </c>
       <c r="X6" t="n">
-        <v>140.0452</v>
+        <v>45.07205</v>
       </c>
       <c r="Y6" t="n">
-        <v>386.3998</v>
+        <v>381.5217</v>
       </c>
       <c r="Z6" t="n">
-        <v>149.4762</v>
+        <v>409.409</v>
       </c>
       <c r="AA6" t="n">
-        <v>423.8866</v>
+        <v>446.8056</v>
       </c>
       <c r="AB6" t="n">
-        <v>829.5927</v>
+        <v>200.3346</v>
       </c>
       <c r="AC6" t="n">
-        <v>525.9893</v>
+        <v>429.7361</v>
       </c>
       <c r="AD6" t="n">
-        <v>411.6554</v>
+        <v>590.1577</v>
       </c>
       <c r="AE6" t="n">
-        <v>292.0843</v>
+        <v>400.7928</v>
       </c>
       <c r="AF6" t="n">
-        <v>348404.9</v>
+        <v>3910121</v>
       </c>
       <c r="AG6" t="n">
         <v>10</v>
@@ -1108,94 +1108,94 @@
         <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>629130200</v>
+        <v>335.4654</v>
       </c>
       <c r="D7" t="n">
-        <v>2144239</v>
+        <v>614</v>
       </c>
       <c r="E7" t="n">
-        <v>1233.518</v>
+        <v>0.2980207</v>
       </c>
       <c r="F7" t="n">
-        <v>28.28549</v>
+        <v>65.34947</v>
       </c>
       <c r="G7" t="n">
-        <v>70.67825999999999</v>
+        <v>39.79826</v>
       </c>
       <c r="H7" t="n">
-        <v>29.90937</v>
+        <v>44.23154</v>
       </c>
       <c r="I7" t="n">
-        <v>42.77243</v>
+        <v>53.87765</v>
       </c>
       <c r="J7" t="n">
-        <v>12.28001</v>
+        <v>10.94454</v>
       </c>
       <c r="K7" t="n">
-        <v>236.4845</v>
+        <v>376.0615</v>
       </c>
       <c r="L7" t="n">
-        <v>1352.415</v>
+        <v>1032.007</v>
       </c>
       <c r="M7" t="n">
-        <v>42.38247</v>
+        <v>24.75503</v>
       </c>
       <c r="N7" t="n">
-        <v>13138.75</v>
+        <v>5096332</v>
       </c>
       <c r="O7" t="n">
-        <v>10723.37</v>
+        <v>14310.62</v>
       </c>
       <c r="P7" t="n">
-        <v>3532.35</v>
+        <v>121.2276</v>
       </c>
       <c r="Q7" t="n">
-        <v>5729.34</v>
+        <v>481.2134</v>
       </c>
       <c r="R7" t="n">
-        <v>120.0553</v>
+        <v>412.9659</v>
       </c>
       <c r="S7" t="n">
-        <v>60.80782</v>
+        <v>140.2325</v>
       </c>
       <c r="T7" t="n">
-        <v>1298.477</v>
+        <v>9600.191999999999</v>
       </c>
       <c r="U7" t="n">
-        <v>2614.75</v>
+        <v>3160.17</v>
       </c>
       <c r="V7" t="n">
-        <v>247.5062</v>
+        <v>29.0567</v>
       </c>
       <c r="W7" t="n">
-        <v>118.2991</v>
+        <v>237.139</v>
       </c>
       <c r="X7" t="n">
-        <v>115.3529</v>
+        <v>45.01828</v>
       </c>
       <c r="Y7" t="n">
-        <v>379.0052</v>
+        <v>381.412</v>
       </c>
       <c r="Z7" t="n">
-        <v>117.7447</v>
+        <v>409.4059</v>
       </c>
       <c r="AA7" t="n">
-        <v>402.4682</v>
+        <v>401.127</v>
       </c>
       <c r="AB7" t="n">
-        <v>679.2888</v>
+        <v>200.0005</v>
       </c>
       <c r="AC7" t="n">
-        <v>446.7127</v>
+        <v>417.8813</v>
       </c>
       <c r="AD7" t="n">
-        <v>370.5559</v>
+        <v>589.3015</v>
       </c>
       <c r="AE7" t="n">
-        <v>289.2193</v>
+        <v>385.3237</v>
       </c>
       <c r="AF7" t="n">
-        <v>109990.6</v>
+        <v>3661147</v>
       </c>
       <c r="AG7" t="n">
         <v>10</v>
@@ -1209,94 +1209,94 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>110445200</v>
+        <v>335.4377</v>
       </c>
       <c r="D8" t="n">
-        <v>486702</v>
+        <v>65</v>
       </c>
       <c r="E8" t="n">
-        <v>622.4666</v>
+        <v>0.001027147</v>
       </c>
       <c r="F8" t="n">
-        <v>11.96829</v>
+        <v>63.15317</v>
       </c>
       <c r="G8" t="n">
-        <v>70.65425</v>
+        <v>39.79826</v>
       </c>
       <c r="H8" t="n">
-        <v>29.89379</v>
+        <v>44.2159</v>
       </c>
       <c r="I8" t="n">
-        <v>42.76903</v>
+        <v>53.87764</v>
       </c>
       <c r="J8" t="n">
-        <v>11.98397</v>
+        <v>10.94454</v>
       </c>
       <c r="K8" t="n">
-        <v>236.2118</v>
+        <v>376.0578</v>
       </c>
       <c r="L8" t="n">
-        <v>1349.021</v>
+        <v>1032.007</v>
       </c>
       <c r="M8" t="n">
-        <v>25.72069</v>
+        <v>24.44419</v>
       </c>
       <c r="N8" t="n">
-        <v>13036.77</v>
+        <v>4559838</v>
       </c>
       <c r="O8" t="n">
-        <v>10705.23</v>
+        <v>14049.1</v>
       </c>
       <c r="P8" t="n">
-        <v>2832.639</v>
+        <v>121.057</v>
       </c>
       <c r="Q8" t="n">
-        <v>5061.707</v>
+        <v>445.8789</v>
       </c>
       <c r="R8" t="n">
-        <v>32.53249</v>
+        <v>411.97</v>
       </c>
       <c r="S8" t="n">
-        <v>58.92578</v>
+        <v>139.3188</v>
       </c>
       <c r="T8" t="n">
-        <v>1298.169</v>
+        <v>9593.989</v>
       </c>
       <c r="U8" t="n">
-        <v>1260.841</v>
+        <v>2564.339</v>
       </c>
       <c r="V8" t="n">
-        <v>244.9928</v>
+        <v>26.0011</v>
       </c>
       <c r="W8" t="n">
-        <v>115.1827</v>
+        <v>237.139</v>
       </c>
       <c r="X8" t="n">
-        <v>115.2336</v>
+        <v>45.01378</v>
       </c>
       <c r="Y8" t="n">
-        <v>361.4108</v>
+        <v>381.3537</v>
       </c>
       <c r="Z8" t="n">
-        <v>109.4482</v>
+        <v>409.4059</v>
       </c>
       <c r="AA8" t="n">
-        <v>400.4133</v>
+        <v>397.8941</v>
       </c>
       <c r="AB8" t="n">
-        <v>618.7794</v>
+        <v>200</v>
       </c>
       <c r="AC8" t="n">
-        <v>443.2541</v>
+        <v>417.8812</v>
       </c>
       <c r="AD8" t="n">
-        <v>331.5374</v>
+        <v>584.0365</v>
       </c>
       <c r="AE8" t="n">
-        <v>288.2638</v>
+        <v>384.0355</v>
       </c>
       <c r="AF8" t="n">
-        <v>102671.4</v>
+        <v>3411841</v>
       </c>
       <c r="AG8" t="n">
         <v>10</v>
@@ -1310,94 +1310,94 @@
         <v>40</v>
       </c>
       <c r="C9" t="n">
-        <v>11831330</v>
+        <v>335.4327</v>
       </c>
       <c r="D9" t="n">
-        <v>179266</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
-        <v>264.115</v>
+        <v>5.032042e-06</v>
       </c>
       <c r="F9" t="n">
-        <v>3.42592</v>
+        <v>46.82428</v>
       </c>
       <c r="G9" t="n">
-        <v>70.64232</v>
+        <v>39.79826</v>
       </c>
       <c r="H9" t="n">
-        <v>29.88471</v>
+        <v>44.21249</v>
       </c>
       <c r="I9" t="n">
-        <v>42.76842</v>
+        <v>53.87764</v>
       </c>
       <c r="J9" t="n">
-        <v>11.93955</v>
+        <v>10.94454</v>
       </c>
       <c r="K9" t="n">
-        <v>236.1891</v>
+        <v>376.053</v>
       </c>
       <c r="L9" t="n">
-        <v>1348.883</v>
+        <v>1032.007</v>
       </c>
       <c r="M9" t="n">
-        <v>22.0404</v>
+        <v>24.38483</v>
       </c>
       <c r="N9" t="n">
-        <v>12719.13</v>
+        <v>3593074</v>
       </c>
       <c r="O9" t="n">
-        <v>10664.81</v>
+        <v>14006.06</v>
       </c>
       <c r="P9" t="n">
-        <v>2688.71</v>
+        <v>118.0079</v>
       </c>
       <c r="Q9" t="n">
-        <v>1865.603</v>
+        <v>444.6148</v>
       </c>
       <c r="R9" t="n">
-        <v>20.40423</v>
+        <v>410.6553</v>
       </c>
       <c r="S9" t="n">
-        <v>57.44404</v>
+        <v>139.1401</v>
       </c>
       <c r="T9" t="n">
-        <v>1297.915</v>
+        <v>9590.468000000001</v>
       </c>
       <c r="U9" t="n">
-        <v>553.2016</v>
+        <v>2013.314</v>
       </c>
       <c r="V9" t="n">
-        <v>244.5</v>
+        <v>25.49906</v>
       </c>
       <c r="W9" t="n">
-        <v>113.2065</v>
+        <v>237.139</v>
       </c>
       <c r="X9" t="n">
-        <v>115.2114</v>
+        <v>45.01153</v>
       </c>
       <c r="Y9" t="n">
-        <v>357.8639</v>
+        <v>381.2746</v>
       </c>
       <c r="Z9" t="n">
-        <v>103.302</v>
+        <v>409.4059</v>
       </c>
       <c r="AA9" t="n">
-        <v>399.8053</v>
+        <v>397.8862</v>
       </c>
       <c r="AB9" t="n">
-        <v>527.3261</v>
+        <v>200</v>
       </c>
       <c r="AC9" t="n">
-        <v>419.5403</v>
+        <v>417.8812</v>
       </c>
       <c r="AD9" t="n">
-        <v>306.6095</v>
+        <v>538.8083</v>
       </c>
       <c r="AE9" t="n">
-        <v>285.2003</v>
+        <v>383.0838</v>
       </c>
       <c r="AF9" t="n">
-        <v>98963.99000000001</v>
+        <v>3348130</v>
       </c>
       <c r="AG9" t="n">
         <v>10</v>
@@ -1411,94 +1411,94 @@
         <v>50</v>
       </c>
       <c r="C10" t="n">
-        <v>457585.2</v>
+        <v>335.4271</v>
       </c>
       <c r="D10" t="n">
-        <v>179266</v>
+        <v>25</v>
       </c>
       <c r="E10" t="n">
-        <v>111.3692</v>
+        <v>2.813033e-08</v>
       </c>
       <c r="F10" t="n">
-        <v>1.06231</v>
+        <v>3.608255</v>
       </c>
       <c r="G10" t="n">
-        <v>70.64152</v>
+        <v>39.79826</v>
       </c>
       <c r="H10" t="n">
-        <v>29.87565</v>
+        <v>44.2114</v>
       </c>
       <c r="I10" t="n">
-        <v>42.76839</v>
+        <v>53.87764</v>
       </c>
       <c r="J10" t="n">
-        <v>11.93951</v>
+        <v>10.94454</v>
       </c>
       <c r="K10" t="n">
-        <v>236.182</v>
+        <v>376.0495</v>
       </c>
       <c r="L10" t="n">
-        <v>1348.874</v>
+        <v>1032.007</v>
       </c>
       <c r="M10" t="n">
-        <v>21.88712</v>
+        <v>24.35515</v>
       </c>
       <c r="N10" t="n">
-        <v>12612.97</v>
+        <v>3030631</v>
       </c>
       <c r="O10" t="n">
-        <v>10616.65</v>
+        <v>13981.62</v>
       </c>
       <c r="P10" t="n">
-        <v>321.9612</v>
+        <v>117.8684</v>
       </c>
       <c r="Q10" t="n">
-        <v>1848.224</v>
+        <v>437.5088</v>
       </c>
       <c r="R10" t="n">
-        <v>19.49221</v>
+        <v>409.6952</v>
       </c>
       <c r="S10" t="n">
-        <v>55.87184</v>
+        <v>138.964</v>
       </c>
       <c r="T10" t="n">
-        <v>1296.54</v>
+        <v>9587.528</v>
       </c>
       <c r="U10" t="n">
-        <v>517.9478</v>
+        <v>1795.753</v>
       </c>
       <c r="V10" t="n">
-        <v>242.7872</v>
+        <v>25.32956</v>
       </c>
       <c r="W10" t="n">
-        <v>107.5589</v>
+        <v>118.4555</v>
       </c>
       <c r="X10" t="n">
-        <v>115.195</v>
+        <v>45.01051</v>
       </c>
       <c r="Y10" t="n">
-        <v>356.701</v>
+        <v>340.9954</v>
       </c>
       <c r="Z10" t="n">
-        <v>100.7976</v>
+        <v>409.4059</v>
       </c>
       <c r="AA10" t="n">
-        <v>399.7178</v>
+        <v>397.8862</v>
       </c>
       <c r="AB10" t="n">
-        <v>439.5438</v>
+        <v>200</v>
       </c>
       <c r="AC10" t="n">
-        <v>406.1924</v>
+        <v>415.2786</v>
       </c>
       <c r="AD10" t="n">
-        <v>301.5155</v>
+        <v>410.8879</v>
       </c>
       <c r="AE10" t="n">
-        <v>284.9855</v>
+        <v>382.6354</v>
       </c>
       <c r="AF10" t="n">
-        <v>94946.02</v>
+        <v>2842109</v>
       </c>
       <c r="AG10" t="n">
         <v>10</v>
@@ -1512,94 +1512,94 @@
         <v>60</v>
       </c>
       <c r="C11" t="n">
-        <v>28406.47</v>
+        <v>335.4222</v>
       </c>
       <c r="D11" t="n">
-        <v>178100</v>
+        <v>18</v>
       </c>
       <c r="E11" t="n">
-        <v>65.42025</v>
+        <v>6.400569e-11</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2947086</v>
+        <v>2.862653</v>
       </c>
       <c r="G11" t="n">
-        <v>70.64149</v>
+        <v>39.79826</v>
       </c>
       <c r="H11" t="n">
-        <v>29.86027</v>
+        <v>44.21025</v>
       </c>
       <c r="I11" t="n">
-        <v>42.76838</v>
+        <v>53.87764</v>
       </c>
       <c r="J11" t="n">
-        <v>11.9395</v>
+        <v>10.94454</v>
       </c>
       <c r="K11" t="n">
-        <v>236.1745</v>
+        <v>376.0467</v>
       </c>
       <c r="L11" t="n">
-        <v>1348.872</v>
+        <v>1032.007</v>
       </c>
       <c r="M11" t="n">
-        <v>21.84321</v>
+        <v>24.338</v>
       </c>
       <c r="N11" t="n">
-        <v>12462.48</v>
+        <v>2632355</v>
       </c>
       <c r="O11" t="n">
-        <v>10610.32</v>
+        <v>13953.73</v>
       </c>
       <c r="P11" t="n">
-        <v>311.8298</v>
+        <v>117.684</v>
       </c>
       <c r="Q11" t="n">
-        <v>1672.144</v>
+        <v>433.0859</v>
       </c>
       <c r="R11" t="n">
-        <v>18.29297</v>
+        <v>408.3644</v>
       </c>
       <c r="S11" t="n">
-        <v>55.5067</v>
+        <v>138.8208</v>
       </c>
       <c r="T11" t="n">
-        <v>1272.708</v>
+        <v>9580.804</v>
       </c>
       <c r="U11" t="n">
-        <v>43.37284</v>
+        <v>1624.848</v>
       </c>
       <c r="V11" t="n">
-        <v>242.5731</v>
+        <v>25.32667</v>
       </c>
       <c r="W11" t="n">
-        <v>106.1836</v>
+        <v>106.2642</v>
       </c>
       <c r="X11" t="n">
-        <v>115.192</v>
+        <v>45.00988</v>
       </c>
       <c r="Y11" t="n">
-        <v>347.1314</v>
+        <v>340.9795</v>
       </c>
       <c r="Z11" t="n">
-        <v>100.2184</v>
+        <v>409.4059</v>
       </c>
       <c r="AA11" t="n">
-        <v>399.6418</v>
+        <v>397.8862</v>
       </c>
       <c r="AB11" t="n">
-        <v>409.8248</v>
+        <v>200</v>
       </c>
       <c r="AC11" t="n">
-        <v>405.5293</v>
+        <v>415.2449</v>
       </c>
       <c r="AD11" t="n">
-        <v>300.4934</v>
+        <v>343.0191</v>
       </c>
       <c r="AE11" t="n">
-        <v>284.8034</v>
+        <v>381.7592</v>
       </c>
       <c r="AF11" t="n">
-        <v>92839.42</v>
+        <v>2112640</v>
       </c>
       <c r="AG11" t="n">
         <v>10</v>
@@ -1613,94 +1613,94 @@
         <v>70</v>
       </c>
       <c r="C12" t="n">
-        <v>2646.665</v>
+        <v>335.4163</v>
       </c>
       <c r="D12" t="n">
-        <v>170483</v>
+        <v>17</v>
       </c>
       <c r="E12" t="n">
-        <v>30.46265</v>
+        <v>2.614797e-12</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1032738</v>
+        <v>2.612959</v>
       </c>
       <c r="G12" t="n">
-        <v>48.99013</v>
+        <v>39.79826</v>
       </c>
       <c r="H12" t="n">
-        <v>29.85067</v>
+        <v>44.20915</v>
       </c>
       <c r="I12" t="n">
-        <v>42.76838</v>
+        <v>53.87764</v>
       </c>
       <c r="J12" t="n">
-        <v>11.9395</v>
+        <v>10.94454</v>
       </c>
       <c r="K12" t="n">
-        <v>236.1637</v>
+        <v>376.044</v>
       </c>
       <c r="L12" t="n">
-        <v>1348.872</v>
+        <v>680.2667</v>
       </c>
       <c r="M12" t="n">
-        <v>21.83594</v>
+        <v>24.32238</v>
       </c>
       <c r="N12" t="n">
-        <v>12323.53</v>
+        <v>2149906</v>
       </c>
       <c r="O12" t="n">
-        <v>10580.94</v>
+        <v>13766.46</v>
       </c>
       <c r="P12" t="n">
-        <v>134.6436</v>
+        <v>117.5742</v>
       </c>
       <c r="Q12" t="n">
-        <v>1299.143</v>
+        <v>375.2475</v>
       </c>
       <c r="R12" t="n">
-        <v>17.98952</v>
+        <v>407.6401</v>
       </c>
       <c r="S12" t="n">
-        <v>55.04205</v>
+        <v>138.7762</v>
       </c>
       <c r="T12" t="n">
-        <v>1272.413</v>
+        <v>9576.688</v>
       </c>
       <c r="U12" t="n">
-        <v>43.37229</v>
+        <v>1609.268</v>
       </c>
       <c r="V12" t="n">
-        <v>242.5633</v>
+        <v>25.32539</v>
       </c>
       <c r="W12" t="n">
-        <v>105.1683</v>
+        <v>103.7109</v>
       </c>
       <c r="X12" t="n">
-        <v>115.1894</v>
+        <v>45.00961</v>
       </c>
       <c r="Y12" t="n">
-        <v>345.1565</v>
+        <v>340.9766</v>
       </c>
       <c r="Z12" t="n">
-        <v>100.0492</v>
+        <v>100.1688</v>
       </c>
       <c r="AA12" t="n">
-        <v>399.6289</v>
+        <v>397.8862</v>
       </c>
       <c r="AB12" t="n">
-        <v>387.8387</v>
+        <v>200</v>
       </c>
       <c r="AC12" t="n">
-        <v>405.5143</v>
+        <v>415.2415</v>
       </c>
       <c r="AD12" t="n">
-        <v>300.1055</v>
+        <v>300.0888</v>
       </c>
       <c r="AE12" t="n">
-        <v>284.6865</v>
+        <v>381.6717</v>
       </c>
       <c r="AF12" t="n">
-        <v>86406.77</v>
+        <v>1482965</v>
       </c>
       <c r="AG12" t="n">
         <v>10</v>
@@ -1714,94 +1714,94 @@
         <v>80</v>
       </c>
       <c r="C13" t="n">
-        <v>932.1099</v>
+        <v>335.412</v>
       </c>
       <c r="D13" t="n">
-        <v>163762</v>
+        <v>17</v>
       </c>
       <c r="E13" t="n">
-        <v>16.39638</v>
+        <v>1.705303e-13</v>
       </c>
       <c r="F13" t="n">
-        <v>0.009023882</v>
+        <v>2.460335</v>
       </c>
       <c r="G13" t="n">
-        <v>47.85983</v>
+        <v>39.79826</v>
       </c>
       <c r="H13" t="n">
-        <v>24.62236</v>
+        <v>44.20801</v>
       </c>
       <c r="I13" t="n">
-        <v>42.76838</v>
+        <v>53.87764</v>
       </c>
       <c r="J13" t="n">
-        <v>11.9395</v>
+        <v>10.94454</v>
       </c>
       <c r="K13" t="n">
-        <v>236.1604</v>
+        <v>376.0406</v>
       </c>
       <c r="L13" t="n">
-        <v>1348.872</v>
+        <v>679.5703999999999</v>
       </c>
       <c r="M13" t="n">
-        <v>21.83374</v>
+        <v>24.30914</v>
       </c>
       <c r="N13" t="n">
-        <v>12243.87</v>
+        <v>1925888</v>
       </c>
       <c r="O13" t="n">
-        <v>10575.33</v>
+        <v>12167.6</v>
       </c>
       <c r="P13" t="n">
-        <v>129.9031</v>
+        <v>117.0525</v>
       </c>
       <c r="Q13" t="n">
-        <v>1214.821</v>
+        <v>374.1416</v>
       </c>
       <c r="R13" t="n">
-        <v>17.802</v>
+        <v>406.8242</v>
       </c>
       <c r="S13" t="n">
-        <v>54.73968</v>
+        <v>137.6407</v>
       </c>
       <c r="T13" t="n">
-        <v>1272.262</v>
+        <v>9573.018</v>
       </c>
       <c r="U13" t="n">
-        <v>43.31606</v>
+        <v>1579.846</v>
       </c>
       <c r="V13" t="n">
-        <v>242.56</v>
+        <v>24.34739</v>
       </c>
       <c r="W13" t="n">
-        <v>104.3422</v>
+        <v>103.5704</v>
       </c>
       <c r="X13" t="n">
-        <v>115.1873</v>
+        <v>45.00922</v>
       </c>
       <c r="Y13" t="n">
-        <v>343.2709</v>
+        <v>340.976</v>
       </c>
       <c r="Z13" t="n">
-        <v>100.0093</v>
+        <v>100.0004</v>
       </c>
       <c r="AA13" t="n">
-        <v>399.6198</v>
+        <v>397.8862</v>
       </c>
       <c r="AB13" t="n">
-        <v>355.4188</v>
+        <v>200</v>
       </c>
       <c r="AC13" t="n">
-        <v>405.5113</v>
+        <v>409.9954</v>
       </c>
       <c r="AD13" t="n">
-        <v>300.0119</v>
+        <v>300.0002</v>
       </c>
       <c r="AE13" t="n">
-        <v>284.5123</v>
+        <v>381.6221</v>
       </c>
       <c r="AF13" t="n">
-        <v>81934.11</v>
+        <v>817930.9</v>
       </c>
       <c r="AG13" t="n">
         <v>10</v>
@@ -1815,94 +1815,94 @@
         <v>90</v>
       </c>
       <c r="C14" t="n">
-        <v>517.8348999999999</v>
+        <v>335.4076</v>
       </c>
       <c r="D14" t="n">
-        <v>153181</v>
+        <v>9</v>
       </c>
       <c r="E14" t="n">
-        <v>12.49728</v>
+        <v>5.684342e-14</v>
       </c>
       <c r="F14" t="n">
-        <v>0.004025143</v>
+        <v>2.265413</v>
       </c>
       <c r="G14" t="n">
-        <v>47.76103</v>
+        <v>39.79826</v>
       </c>
       <c r="H14" t="n">
-        <v>24.39997</v>
+        <v>44.20714</v>
       </c>
       <c r="I14" t="n">
-        <v>42.76838</v>
+        <v>53.87764</v>
       </c>
       <c r="J14" t="n">
-        <v>11.9395</v>
+        <v>10.94454</v>
       </c>
       <c r="K14" t="n">
-        <v>236.1576</v>
+        <v>376.0372</v>
       </c>
       <c r="L14" t="n">
-        <v>1348.872</v>
+        <v>679.5703999999999</v>
       </c>
       <c r="M14" t="n">
-        <v>21.83285</v>
+        <v>24.29526</v>
       </c>
       <c r="N14" t="n">
-        <v>12130.65</v>
+        <v>1700227</v>
       </c>
       <c r="O14" t="n">
-        <v>10527.67</v>
+        <v>12119.03</v>
       </c>
       <c r="P14" t="n">
-        <v>129.5997</v>
+        <v>111.0181</v>
       </c>
       <c r="Q14" t="n">
-        <v>1064.229</v>
+        <v>364.6665</v>
       </c>
       <c r="R14" t="n">
-        <v>17.05763</v>
+        <v>406.2466</v>
       </c>
       <c r="S14" t="n">
-        <v>54.62004</v>
+        <v>137.6399</v>
       </c>
       <c r="T14" t="n">
-        <v>1271.493</v>
+        <v>9567.870999999999</v>
       </c>
       <c r="U14" t="n">
-        <v>43.30514</v>
+        <v>1369.213</v>
       </c>
       <c r="V14" t="n">
-        <v>242.445</v>
+        <v>24.3228</v>
       </c>
       <c r="W14" t="n">
-        <v>103.4434</v>
+        <v>103.4933</v>
       </c>
       <c r="X14" t="n">
-        <v>115.1806</v>
+        <v>45.00921</v>
       </c>
       <c r="Y14" t="n">
-        <v>342.0041</v>
+        <v>340.976</v>
       </c>
       <c r="Z14" t="n">
-        <v>100.004</v>
+        <v>100</v>
       </c>
       <c r="AA14" t="n">
-        <v>399.6156</v>
+        <v>397.8862</v>
       </c>
       <c r="AB14" t="n">
-        <v>315.8983</v>
+        <v>200</v>
       </c>
       <c r="AC14" t="n">
-        <v>405.5084</v>
+        <v>408.9318</v>
       </c>
       <c r="AD14" t="n">
-        <v>300.0064</v>
+        <v>300</v>
       </c>
       <c r="AE14" t="n">
-        <v>284.4438</v>
+        <v>381.385</v>
       </c>
       <c r="AF14" t="n">
-        <v>75916.91</v>
+        <v>817580.8</v>
       </c>
       <c r="AG14" t="n">
         <v>10</v>
@@ -1916,94 +1916,94 @@
         <v>100</v>
       </c>
       <c r="C15" t="n">
-        <v>489.7132</v>
+        <v>335.404</v>
       </c>
       <c r="D15" t="n">
-        <v>112515</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>7.064827</v>
+        <v>5.684342e-14</v>
       </c>
       <c r="F15" t="n">
-        <v>0.002380647</v>
+        <v>2.139565</v>
       </c>
       <c r="G15" t="n">
-        <v>47.7585</v>
+        <v>39.79826</v>
       </c>
       <c r="H15" t="n">
-        <v>24.38846</v>
+        <v>44.20631</v>
       </c>
       <c r="I15" t="n">
-        <v>42.76838</v>
+        <v>53.87764</v>
       </c>
       <c r="J15" t="n">
-        <v>11.9395</v>
+        <v>10.94454</v>
       </c>
       <c r="K15" t="n">
-        <v>236.1532</v>
+        <v>376.0342</v>
       </c>
       <c r="L15" t="n">
-        <v>1348.872</v>
+        <v>679.5703999999999</v>
       </c>
       <c r="M15" t="n">
-        <v>21.83255</v>
+        <v>24.28025</v>
       </c>
       <c r="N15" t="n">
-        <v>12033.63</v>
+        <v>1559210</v>
       </c>
       <c r="O15" t="n">
-        <v>10501.63</v>
+        <v>12093.79</v>
       </c>
       <c r="P15" t="n">
-        <v>114.7644</v>
+        <v>105.8206</v>
       </c>
       <c r="Q15" t="n">
-        <v>1055.234</v>
+        <v>363.6583</v>
       </c>
       <c r="R15" t="n">
-        <v>16.50723</v>
+        <v>405.6899</v>
       </c>
       <c r="S15" t="n">
-        <v>54.60367</v>
+        <v>137.5972</v>
       </c>
       <c r="T15" t="n">
-        <v>1271.255</v>
+        <v>9557.436</v>
       </c>
       <c r="U15" t="n">
-        <v>43.30259</v>
+        <v>1293.061</v>
       </c>
       <c r="V15" t="n">
-        <v>242.4126</v>
+        <v>24.3228</v>
       </c>
       <c r="W15" t="n">
-        <v>102.7996</v>
+        <v>103.259</v>
       </c>
       <c r="X15" t="n">
-        <v>115.1799</v>
+        <v>45.00917</v>
       </c>
       <c r="Y15" t="n">
-        <v>341.1999</v>
+        <v>340.976</v>
       </c>
       <c r="Z15" t="n">
-        <v>100.0021</v>
+        <v>100</v>
       </c>
       <c r="AA15" t="n">
-        <v>399.6146</v>
+        <v>397.8862</v>
       </c>
       <c r="AB15" t="n">
-        <v>300.9062</v>
+        <v>200</v>
       </c>
       <c r="AC15" t="n">
-        <v>405.5052</v>
+        <v>407.1154</v>
       </c>
       <c r="AD15" t="n">
-        <v>300.0035</v>
+        <v>300</v>
       </c>
       <c r="AE15" t="n">
-        <v>284.4255</v>
+        <v>381.2699</v>
       </c>
       <c r="AF15" t="n">
-        <v>75120.06</v>
+        <v>817579.1</v>
       </c>
       <c r="AG15" t="n">
         <v>10</v>

</xml_diff>